<commit_message>
edit traceabilityMatrix (delete requirements out of scope and non-functional)
</commit_message>
<xml_diff>
--- a/Docs/Use-cases/TraceabilityMatrix3.xlsx
+++ b/Docs/Use-cases/TraceabilityMatrix3.xlsx
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:BP59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:68" ht="93.75">
+    <row r="7" spans="1:68" ht="75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" ht="94.5" thickBot="1">
+    <row r="21" spans="1:5" ht="75.75" thickBot="1">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" ht="57" thickBot="1">
+    <row r="27" spans="1:5" ht="38.25" thickBot="1">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" ht="94.5" thickBot="1">
+    <row r="31" spans="1:5" ht="75.75" thickBot="1">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="E52" s="23"/>
     </row>
-    <row r="53" spans="1:5" ht="57" thickBot="1">
+    <row r="53" spans="1:5" ht="38.25" thickBot="1">
       <c r="A53" s="8">
         <v>52</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="E54" s="23"/>
     </row>
-    <row r="55" spans="1:5" ht="131.25">
+    <row r="55" spans="1:5" ht="112.5">
       <c r="A55" s="8">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Test cases, sequences, strategy & refreshed tracebility matrix
</commit_message>
<xml_diff>
--- a/Docs/Use-cases/TraceabilityMatrix3.xlsx
+++ b/Docs/Use-cases/TraceabilityMatrix3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="0">Лист1!$K$14</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="182">
   <si>
     <t>#</t>
   </si>
@@ -445,31 +445,6 @@
     <t>WIND.UC.009 WIND.UC.014 WIND.UC.015 WIND.UC.016</t>
   </si>
   <si>
-    <r>
-      <t>WIND.UC.010</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>─</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WIND.UC.016</t>
-    </r>
-  </si>
-  <si>
     <t>WIND.UC.004 WIND.UC.005 WIND.UC.006</t>
   </si>
   <si>
@@ -483,9 +458,6 @@
   </si>
   <si>
     <t>WIND.UC.011  WIND.UC.014</t>
-  </si>
-  <si>
-    <t>WIND.UC.0112 WIND.UC.016</t>
   </si>
   <si>
     <t>WIND.UC.014 WIND.UC.016</t>
@@ -536,6 +508,12 @@
     </r>
   </si>
   <si>
+    <t>Test-case ID</t>
+  </si>
+  <si>
+    <t>WIND.TC.001</t>
+  </si>
+  <si>
     <r>
       <t>WIND.UC.001</t>
     </r>
@@ -547,15 +525,145 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>─WIND.UC.021</t>
+      <t>─ WIND.UC.021</t>
     </r>
+  </si>
+  <si>
+    <t>WIND.TC.003</t>
+  </si>
+  <si>
+    <t>WIND.TC.004 WIND.TC.005 WIND.TC.006</t>
+  </si>
+  <si>
+    <t>WIND.UC.007 WIND.UC.010</t>
+  </si>
+  <si>
+    <r>
+      <t>WIND.UC.007, WIND.UC.010</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">─ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WIND.UC.016</t>
+    </r>
+  </si>
+  <si>
+    <t>WIND.TC.008</t>
+  </si>
+  <si>
+    <t>WIND.TC.009</t>
+  </si>
+  <si>
+    <t>WIND.TC.007 WIND.TC.010-WIND.TC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.010</t>
+  </si>
+  <si>
+    <t>WIND.TC.010-WIND.TC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.007 WIND.TC.010</t>
+  </si>
+  <si>
+    <t>WIND.UC.011 WIND.UC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.011</t>
+  </si>
+  <si>
+    <t>WIND.TC.010 WIND.TC.011 WIND.TC.012 WIND.TC.013</t>
+  </si>
+  <si>
+    <t>WIND.TC.009 WIND.TC.014</t>
+  </si>
+  <si>
+    <t>WIND.TC.014</t>
+  </si>
+  <si>
+    <t>WIND.TC.009 WIND.TC.010 WIND.TC.011 WIND.TC.014</t>
+  </si>
+  <si>
+    <t>WIND.TC.015</t>
+  </si>
+  <si>
+    <t>WIND.TC.011 WIND.TC.014</t>
+  </si>
+  <si>
+    <t>WIND.TC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.009 WIND.TC.014 WIND.TC.015 WIND.TC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.011 WIND.TC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.014 WIND.TC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.012 WIND.TC.016</t>
+  </si>
+  <si>
+    <t>WIND.TC.017</t>
+  </si>
+  <si>
+    <t>WIND.TC.018  WIND.TC.019 WIND.TC.020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIND.TC.018  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIND.TC.019 </t>
+  </si>
+  <si>
+    <t>WIND.TC.021</t>
+  </si>
+  <si>
+    <t>WIND.TC.020</t>
+  </si>
+  <si>
+    <r>
+      <t>WIND.TC.001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>─ WIND.TC.022</t>
+    </r>
+  </si>
+  <si>
+    <t>WIND.TC.001 WIND.TC.002 WIND.TC.022</t>
+  </si>
+  <si>
+    <t>WIND.TC.002 WIND.TC.022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,7 +744,19 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -644,7 +764,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -755,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,12 +894,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -811,9 +924,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -844,17 +954,35 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <font>
         <b val="0"/>
@@ -868,6 +996,32 @@
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -940,19 +1094,6 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -964,14 +1105,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:E59" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E59"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="4"/>
-    <tableColumn id="2" name="req##" dataDxfId="3"/>
-    <tableColumn id="3" name="Requirement description" dataDxfId="2"/>
-    <tableColumn id="4" name="Use-case ID" dataDxfId="1"/>
-    <tableColumn id="5" name="Comments" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:F59" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A1:F59">
+    <filterColumn colId="5"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" name="#" dataDxfId="6"/>
+    <tableColumn id="2" name="req##" dataDxfId="5"/>
+    <tableColumn id="3" name="Requirement description" dataDxfId="4"/>
+    <tableColumn id="4" name="Use-case ID" dataDxfId="3"/>
+    <tableColumn id="5" name="Test-case ID" dataDxfId="0"/>
+    <tableColumn id="6" name="Comments" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1264,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BP59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1273,9 +1417,10 @@
     <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="43.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35" style="1" customWidth="1"/>
-    <col min="6" max="51" width="9.140625" style="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="1" customWidth="1"/>
+    <col min="7" max="51" width="9.140625" style="1"/>
     <col min="52" max="52" width="31.140625" style="1" customWidth="1"/>
     <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1293,10 +1438,12 @@
       <c r="D1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1370,11 +1517,13 @@
       <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="3"/>
+      <c r="D2" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="32"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1448,10 +1597,13 @@
       <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:68" ht="47.25" customHeight="1">
       <c r="A4" s="8">
@@ -1463,10 +1615,13 @@
       <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:68" ht="51.75" customHeight="1">
       <c r="A5" s="8">
@@ -1478,816 +1633,981 @@
       <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:68" ht="57" thickBot="1">
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:68" ht="75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="11"/>
+      <c r="D7" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:68" ht="67.5" customHeight="1" thickBot="1">
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:68" ht="57" thickBot="1">
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:68" ht="57" thickBot="1">
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" spans="1:68" ht="57" thickBot="1">
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:68" ht="57" thickBot="1">
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:68" ht="57" thickBot="1">
       <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:68" ht="75.75" thickBot="1">
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="31"/>
     </row>
     <row r="15" spans="1:68" ht="38.25" thickBot="1">
       <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:68" ht="70.5" customHeight="1" thickBot="1">
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" ht="57" thickBot="1">
+      <c r="E16" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="1:6" ht="57" thickBot="1">
       <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" ht="94.5" thickBot="1">
+      <c r="E17" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:6" ht="94.5" thickBot="1">
       <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" ht="113.25" thickBot="1">
+      <c r="E18" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="19" spans="1:6" ht="113.25" thickBot="1">
       <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" ht="115.5" customHeight="1" thickBot="1">
+      <c r="E19" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="1:6" ht="115.5" customHeight="1" thickBot="1">
       <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" ht="75.75" thickBot="1">
+      <c r="E20" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:6" ht="94.5" thickBot="1">
       <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" ht="78.75" customHeight="1" thickBot="1">
+      <c r="E21" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="31"/>
+    </row>
+    <row r="22" spans="1:6" ht="78.75" customHeight="1" thickBot="1">
       <c r="A22" s="8">
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" ht="57" thickBot="1">
+      <c r="E22" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="31"/>
+    </row>
+    <row r="23" spans="1:6" ht="57" thickBot="1">
       <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" ht="64.5" customHeight="1" thickBot="1">
+      <c r="E23" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="31"/>
+    </row>
+    <row r="24" spans="1:6" ht="64.5" customHeight="1" thickBot="1">
       <c r="A24" s="8">
         <v>23</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:5" ht="57" thickBot="1">
+      <c r="E24" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="31"/>
+    </row>
+    <row r="25" spans="1:6" ht="57" thickBot="1">
       <c r="A25" s="8">
         <v>24</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:5" ht="45.75" customHeight="1" thickBot="1">
+      <c r="E25" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" s="31"/>
+    </row>
+    <row r="26" spans="1:6" ht="45.75" customHeight="1" thickBot="1">
       <c r="A26" s="8">
         <v>25</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" ht="38.25" thickBot="1">
+      <c r="E26" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="31"/>
+    </row>
+    <row r="27" spans="1:6" ht="38.25" thickBot="1">
       <c r="A27" s="8">
         <v>26</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="1:5" ht="113.25" thickBot="1">
+      <c r="E27" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" s="31"/>
+    </row>
+    <row r="28" spans="1:6" ht="113.25" thickBot="1">
       <c r="A28" s="8">
         <v>27</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="1:5" ht="188.25" thickBot="1">
+      <c r="D28" s="17"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="31"/>
+    </row>
+    <row r="29" spans="1:6" ht="188.25" thickBot="1">
       <c r="A29" s="8">
         <v>28</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="1:5" ht="111" customHeight="1" thickBot="1">
+      <c r="E29" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="31"/>
+    </row>
+    <row r="30" spans="1:6" ht="111" customHeight="1" thickBot="1">
       <c r="A30" s="8">
         <v>29</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31" spans="1:5" ht="75.75" thickBot="1">
+      <c r="E30" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" s="31"/>
+    </row>
+    <row r="31" spans="1:6" ht="94.5" thickBot="1">
       <c r="A31" s="8">
         <v>30</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="1:5" ht="187.5">
+      <c r="D31" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="F31" s="31"/>
+    </row>
+    <row r="32" spans="1:6" ht="187.5">
       <c r="A32" s="8">
         <v>31</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="1:5" ht="75.75" thickBot="1">
+      <c r="D32" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="31"/>
+    </row>
+    <row r="33" spans="1:6" ht="75.75" thickBot="1">
       <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" ht="106.5" customHeight="1" thickBot="1">
+      <c r="D33" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="31"/>
+    </row>
+    <row r="34" spans="1:6" ht="106.5" customHeight="1" thickBot="1">
       <c r="A34" s="8">
         <v>33</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="23"/>
-    </row>
-    <row r="35" spans="1:5" ht="57" thickBot="1">
+      <c r="D34" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="1:6" ht="57" thickBot="1">
       <c r="A35" s="8">
         <v>34</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" s="23"/>
-    </row>
-    <row r="36" spans="1:5" ht="113.25" thickBot="1">
+      <c r="D35" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" s="31"/>
+    </row>
+    <row r="36" spans="1:6" ht="113.25" thickBot="1">
       <c r="A36" s="8">
         <v>35</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="23"/>
-    </row>
-    <row r="37" spans="1:5" ht="132" thickBot="1">
+      <c r="D36" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="F36" s="31"/>
+    </row>
+    <row r="37" spans="1:6" ht="132" thickBot="1">
       <c r="A37" s="8">
         <v>36</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="E37" s="23"/>
-    </row>
-    <row r="38" spans="1:5" ht="94.5" thickBot="1">
+      <c r="D37" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="31"/>
+    </row>
+    <row r="38" spans="1:6" ht="94.5" thickBot="1">
       <c r="A38" s="8">
         <v>37</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="E38" s="23"/>
-    </row>
-    <row r="39" spans="1:5" ht="215.25" customHeight="1" thickBot="1">
+      <c r="E38" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F38" s="31"/>
+    </row>
+    <row r="39" spans="1:6" ht="215.25" customHeight="1" thickBot="1">
       <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="23"/>
-    </row>
-    <row r="40" spans="1:5" ht="94.5" thickBot="1">
+      <c r="D39" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="F39" s="31"/>
+    </row>
+    <row r="40" spans="1:6" ht="94.5" thickBot="1">
       <c r="A40" s="8">
         <v>39</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="32" t="s">
+      <c r="D40" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="E40" s="23"/>
-    </row>
-    <row r="41" spans="1:5" ht="69" customHeight="1" thickBot="1">
+      <c r="E40" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="31"/>
+    </row>
+    <row r="41" spans="1:6" ht="69" customHeight="1" thickBot="1">
       <c r="A41" s="8">
         <v>40</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="D41" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="23"/>
-    </row>
-    <row r="42" spans="1:5" ht="44.25" customHeight="1" thickBot="1">
+      <c r="E41" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F41" s="31"/>
+    </row>
+    <row r="42" spans="1:6" ht="44.25" customHeight="1" thickBot="1">
       <c r="A42" s="8">
         <v>41</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="32"/>
-      <c r="E42" s="23"/>
-    </row>
-    <row r="43" spans="1:5" ht="38.25" thickBot="1">
+      <c r="D42" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F42" s="31"/>
+    </row>
+    <row r="43" spans="1:6" ht="38.25" thickBot="1">
       <c r="A43" s="8">
         <v>42</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="32" t="s">
+      <c r="D43" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E43" s="23"/>
-    </row>
-    <row r="44" spans="1:5" ht="38.25" thickBot="1">
+      <c r="E43" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F43" s="31"/>
+    </row>
+    <row r="44" spans="1:6" ht="38.25" thickBot="1">
       <c r="A44" s="8">
         <v>43</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C44" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="E44" s="23"/>
-    </row>
-    <row r="45" spans="1:5" ht="38.25" thickBot="1">
+      <c r="D44" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="F44" s="31"/>
+    </row>
+    <row r="45" spans="1:6" ht="38.25" thickBot="1">
       <c r="A45" s="8">
         <v>44</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D45" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="E45" s="23"/>
-    </row>
-    <row r="46" spans="1:5" ht="57" thickBot="1">
+      <c r="D45" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="F45" s="31"/>
+    </row>
+    <row r="46" spans="1:6" ht="57" thickBot="1">
       <c r="A46" s="8">
         <v>45</v>
       </c>
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D46" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="E46" s="23"/>
-    </row>
-    <row r="47" spans="1:5" ht="57" thickBot="1">
+      <c r="D46" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="31"/>
+    </row>
+    <row r="47" spans="1:6" ht="57" thickBot="1">
       <c r="A47" s="8">
         <v>46</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D47" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" s="23"/>
-    </row>
-    <row r="48" spans="1:5" ht="57" thickBot="1">
+      <c r="D47" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="F47" s="31"/>
+    </row>
+    <row r="48" spans="1:6" ht="57" thickBot="1">
       <c r="A48" s="8">
         <v>47</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="D48" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="E48" s="23"/>
-    </row>
-    <row r="49" spans="1:5" ht="57" thickBot="1">
+      <c r="D48" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="F48" s="31"/>
+    </row>
+    <row r="49" spans="1:6" ht="57" thickBot="1">
       <c r="A49" s="8">
         <v>48</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D49" s="32" t="s">
+      <c r="D49" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="E49" s="23"/>
-    </row>
-    <row r="50" spans="1:5" ht="38.25" thickBot="1">
+      <c r="E49" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="F49" s="31"/>
+    </row>
+    <row r="50" spans="1:6" ht="38.25" thickBot="1">
       <c r="A50" s="8">
         <v>49</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D50" s="32" t="s">
+      <c r="D50" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="E50" s="23"/>
-    </row>
-    <row r="51" spans="1:5" ht="57" thickBot="1">
+      <c r="E50" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" s="31"/>
+    </row>
+    <row r="51" spans="1:6" ht="57" thickBot="1">
       <c r="A51" s="8">
         <v>50</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D51" s="32" t="s">
+      <c r="D51" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="23"/>
-    </row>
-    <row r="52" spans="1:5" ht="66" customHeight="1" thickBot="1">
+      <c r="E51" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="F51" s="31"/>
+    </row>
+    <row r="52" spans="1:6" ht="66" customHeight="1" thickBot="1">
       <c r="A52" s="8">
         <v>51</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="32" t="s">
+      <c r="D52" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="E52" s="23"/>
-    </row>
-    <row r="53" spans="1:5" ht="38.25" thickBot="1">
+      <c r="E52" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F52" s="31"/>
+    </row>
+    <row r="53" spans="1:6" ht="57" thickBot="1">
       <c r="A53" s="8">
         <v>52</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C53" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="D53" s="33" t="s">
+      <c r="D53" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E53" s="23"/>
-    </row>
-    <row r="54" spans="1:5" ht="84" customHeight="1" thickBot="1">
+      <c r="E53" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F53" s="31"/>
+    </row>
+    <row r="54" spans="1:6" ht="84" customHeight="1" thickBot="1">
       <c r="A54" s="8">
         <v>53</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C54" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="32" t="s">
+      <c r="D54" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="E54" s="23"/>
-    </row>
-    <row r="55" spans="1:5" ht="112.5">
+      <c r="E54" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F54" s="31"/>
+    </row>
+    <row r="55" spans="1:6" ht="112.5">
       <c r="A55" s="8">
         <v>54</v>
       </c>
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="D55" s="33" t="s">
+      <c r="D55" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="E55" s="23"/>
-    </row>
-    <row r="56" spans="1:5" ht="113.25" thickBot="1">
+      <c r="E55" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="F55" s="31"/>
+    </row>
+    <row r="56" spans="1:6" ht="113.25" thickBot="1">
       <c r="A56" s="8">
         <v>55</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="B56" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="E56" s="23"/>
-    </row>
-    <row r="57" spans="1:5" ht="117" customHeight="1" thickBot="1">
+      <c r="E56" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F56" s="31"/>
+    </row>
+    <row r="57" spans="1:6" ht="117" customHeight="1" thickBot="1">
       <c r="A57" s="8">
         <v>56</v>
       </c>
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="E57" s="23"/>
-    </row>
-    <row r="58" spans="1:5" ht="75">
+      <c r="E57" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="F57" s="31"/>
+    </row>
+    <row r="58" spans="1:6" ht="75">
       <c r="A58" s="8">
         <v>57</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="30" t="s">
+      <c r="C58" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="D58" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="E58" s="23"/>
-    </row>
-    <row r="59" spans="1:5" ht="57" thickBot="1">
+      <c r="E58" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="F58" s="31"/>
+    </row>
+    <row r="59" spans="1:6" ht="57" thickBot="1">
       <c r="A59" s="8">
         <v>58</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B59" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C59" s="28" t="s">
+      <c r="C59" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="32" t="s">
+      <c r="D59" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="E59" s="23"/>
+      <c r="E59" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F59" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>